<commit_message>
Corregir funciones de importación Excel - limpiar datos previos y mejorar detección de columnas
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andru\Desktop\AsociacionBasket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC57C77B-5A98-49AD-BAB7-138D27516BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D072D0C0-06EF-40FB-A997-7D498F0B6230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58503C79-47D2-4093-9E9D-079D5ABF11FC}"/>
   </bookViews>
@@ -35,9 +35,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>equipo1</t>
+  </si>
+  <si>
+    <t>equipo2</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>cancha</t>
+  </si>
+  <si>
+    <t>Titanes</t>
+  </si>
+  <si>
+    <t>Águilas</t>
+  </si>
+  <si>
+    <t>Cancha Central</t>
+  </si>
+  <si>
+    <t>Leones</t>
+  </si>
+  <si>
+    <t>Dragones</t>
+  </si>
+  <si>
+    <t>Cancha Norte</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +83,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF181818"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +127,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +495,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A270CF8E-D72F-4704-8363-6650A73C74A7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45976</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45977</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.8125</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>